<commit_message>
list of screened papers
</commit_message>
<xml_diff>
--- a/data/from_readers/ReviewedByALLuza/Descriptors_crosstaxa_review_SFLOETER_ALLUZA.xlsx
+++ b/data/from_readers/ReviewedByALLuza/Descriptors_crosstaxa_review_SFLOETER_ALLUZA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topoa\Dropbox\ReefSyn\wg_syn\data\from_readers\ReviewedByALLuza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E27EE0B-9D43-4ADC-AA02-D7B8065F4037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53002CC6-348D-4A72-9BF3-2DFE7D9D6386}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfPapers" sheetId="1" r:id="rId1"/>
@@ -1424,7 +1424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2739,7 +2741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD1162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3:B258"/>
     </sheetView>

</xml_diff>